<commit_message>
SQL Join parents E-Mail
</commit_message>
<xml_diff>
--- a/Burndownchart_Mondpichl_Sprint2.xlsx
+++ b/Burndownchart_Mondpichl_Sprint2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\josip\Documents\5AHWII\SWP\CCC_Projekt\Ferienspass\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE959A9F-9BEE-49A6-A083-3DFAE5068E84}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A82B4EFF-8EE1-414B-B430-0333E9A720CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -967,7 +967,7 @@
                   <c:v>77.005128205128202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>22.628377504848096</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -1504,7 +1504,7 @@
                   <c:v>77.005128205128202</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>#N/A</c:v>
+                  <c:v>22.628377504848096</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>#N/A</c:v>
@@ -3488,7 +3488,7 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="C13" sqref="C13"/>
+      <selection pane="bottomRight" activeCell="Q8" sqref="Q8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3671,7 +3671,10 @@
         <f>B8/(1+1.5+5)*1</f>
         <v>4.5333333333333332</v>
       </c>
-      <c r="D8" s="20"/>
+      <c r="D8" s="19">
+        <f>B8/(7+2)*6</f>
+        <v>22.666666666666664</v>
+      </c>
       <c r="E8" s="19"/>
       <c r="F8" s="20"/>
       <c r="G8" s="19"/>
@@ -3682,11 +3685,11 @@
       <c r="L8" s="20"/>
       <c r="M8" s="27">
         <f t="shared" ref="M8:M37" si="0">B8-SUM(C8:L8)</f>
-        <v>29.466666666666669</v>
+        <v>6.8000000000000043</v>
       </c>
       <c r="N8" s="17">
         <f t="shared" ref="N8:N38" si="1">IFERROR(1-(M8/B8),"")</f>
-        <v>0.1333333333333333</v>
+        <v>0.79999999999999982</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
@@ -3699,7 +3702,9 @@
       <c r="C9" s="19">
         <v>0</v>
       </c>
-      <c r="D9" s="23"/>
+      <c r="D9" s="19">
+        <v>0</v>
+      </c>
       <c r="E9" s="22"/>
       <c r="F9" s="23"/>
       <c r="G9" s="22"/>
@@ -3728,7 +3733,10 @@
         <f>B10/(2+1+3.5)*2</f>
         <v>6.4615384615384617</v>
       </c>
-      <c r="D10" s="23"/>
+      <c r="D10" s="19">
+        <f>B10/(6.5+1+1)*5</f>
+        <v>12.352941176470589</v>
+      </c>
       <c r="E10" s="22"/>
       <c r="F10" s="23"/>
       <c r="G10" s="22"/>
@@ -3739,11 +3747,11 @@
       <c r="L10" s="23"/>
       <c r="M10" s="28">
         <f t="shared" si="0"/>
-        <v>14.538461538461538</v>
+        <v>2.1855203619909496</v>
       </c>
       <c r="N10" s="17">
         <f t="shared" si="1"/>
-        <v>0.30769230769230771</v>
+        <v>0.89592760180995479</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.65">
@@ -3757,7 +3765,10 @@
         <f>B11/(2+2+2)*2</f>
         <v>7</v>
       </c>
-      <c r="D11" s="23"/>
+      <c r="D11" s="19">
+        <f>B11/(7+2+0)*6</f>
+        <v>14</v>
+      </c>
       <c r="E11" s="22"/>
       <c r="F11" s="23"/>
       <c r="G11" s="22"/>
@@ -3768,11 +3779,11 @@
       <c r="L11" s="23"/>
       <c r="M11" s="28">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>0</v>
       </c>
       <c r="N11" s="17">
         <f t="shared" si="1"/>
-        <v>0.33333333333333337</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.6">
@@ -3786,7 +3797,10 @@
         <f>B12/(5+2+0)*5</f>
         <v>15</v>
       </c>
-      <c r="D12" s="23"/>
+      <c r="D12" s="19">
+        <f>C12/(10+2+2)*5</f>
+        <v>5.3571428571428568</v>
+      </c>
       <c r="E12" s="22"/>
       <c r="F12" s="23"/>
       <c r="G12" s="22"/>
@@ -3797,11 +3811,11 @@
       <c r="L12" s="23"/>
       <c r="M12" s="28">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>0.64285714285714235</v>
       </c>
       <c r="N12" s="17">
         <f t="shared" si="1"/>
-        <v>0.7142857142857143</v>
+        <v>0.96938775510204089</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="30" customHeight="1" x14ac:dyDescent="0.6">
@@ -4366,9 +4380,9 @@
         <f>IFERROR(IF(B38-SUM(C8:C37)=B38,NA(),B38-SUM(C8:C37)),NA())</f>
         <v>77.005128205128202</v>
       </c>
-      <c r="D38" s="11" t="e">
+      <c r="D38" s="11">
         <f t="shared" ref="D38:L38" si="2">IFERROR(IF(C38-SUM(D8:D37)=C38,NA(),C38-SUM(D8:D37)),NA())</f>
-        <v>#N/A</v>
+        <v>22.628377504848096</v>
       </c>
       <c r="E38" s="11" t="e">
         <f t="shared" si="2"/>
@@ -4404,11 +4418,11 @@
       </c>
       <c r="M38" s="35">
         <f>SUM(M8:M37)</f>
-        <v>77.005128205128216</v>
+        <v>22.628377504848096</v>
       </c>
       <c r="N38" s="30">
         <f t="shared" si="1"/>
-        <v>0.2999533799533799</v>
+        <v>0.79428747722865367</v>
       </c>
     </row>
     <row r="39" spans="1:14" ht="17.25" thickBot="1" x14ac:dyDescent="0.65">
@@ -4526,7 +4540,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="AA28" sqref="AA28"/>
+      <selection activeCell="C48" sqref="C48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>